<commit_message>
Updating IG with new URL
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-ARTStartType.xlsx
+++ b/output/StructureDefinition-ARTStartType.xlsx
@@ -212,7 +212,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://example.org/fhir/fish/StructureDefinition/ARTStartType</t>
+    <t>http://regenstrief.org/fhir/StructureDefinition/ARTStartType</t>
   </si>
   <si>
     <t>N/A</t>
@@ -248,7 +248,7 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>http://example.org/fhir/fish/ValueSet/ARTStartTypeValues</t>
+    <t>http://regenstrief.org/fhir/ValueSet/ARTStartTypeValues</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="53.9140625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="52.0390625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>

</xml_diff>